<commit_message>
update renv.locks and ph_integrated related project
</commit_message>
<xml_diff>
--- a/inst/ph_integrated_tables/resources/ph_integrated_template.xlsx
+++ b/inst/ph_integrated_tables/resources/ph_integrated_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Desktop\ph_integrated_tables\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Desktop\git\impactR4PHU\inst\ph_integrated_tables\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A135FB-6776-4FCB-A9C9-7ECF3C81F968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028A9A9B-2231-44FC-B8BC-5E776486CF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="3" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t>Emergency Coping Strategies</t>
   </si>
   <si>
-    <t>Improved Water</t>
-  </si>
-  <si>
     <t>% of Hhwithout access to a sufficient quantity of drinking water (often and always)</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>&lt;=20%</t>
+  </si>
+  <si>
+    <t>Improved Water Source</t>
   </si>
 </sst>
 </file>
@@ -470,15 +470,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -513,6 +504,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -858,38 +858,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94DF9366-7747-453F-9674-901A9D58CFDA}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="12"/>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="9"/>
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="9" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="11"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="24"/>
       <c r="O1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="223.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>20</v>
+      <c r="A2" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -919,252 +919,252 @@
         <v>11</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="O2" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="D3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="L3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="16" t="s">
+      <c r="N3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="15" t="s">
-        <v>23</v>
+      <c r="O3" s="12" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="D4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="19" t="s">
+      <c r="F4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="15" t="s">
+      <c r="L4" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" s="15" t="s">
-        <v>29</v>
+      <c r="M4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="C5" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="D5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="19" t="s">
+      <c r="F5" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="N5" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="O5" s="15" t="s">
-        <v>35</v>
+      <c r="L5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="D6" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="19" t="s">
+      <c r="F6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="M6" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="N6" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="O6" s="15" t="s">
-        <v>40</v>
+      <c r="L6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="C7" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="D7" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="22" t="s">
+      <c r="F7" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="J7" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="K7" s="21" t="s">
+      <c r="L7" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="L7" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="M7" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="N7" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="O7" s="21" t="s">
-        <v>45</v>
+      <c r="M7" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" s="18" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1181,43 +1181,43 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:P2"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="9" t="s">
+      <c r="A1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="9" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="11"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="24"/>
       <c r="P1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="223.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -1247,19 +1247,19 @@
         <v>11</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="P2" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1293,44 +1293,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88864FF9-E532-4B33-9CCF-3B9FDE69E91E}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3:T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="9" t="s">
+      <c r="A1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="9" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="11"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="24"/>
       <c r="P1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="223.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -1360,19 +1360,19 @@
         <v>11</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="P2" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update add_iycf and some changes to teh ph integrated tables
</commit_message>
<xml_diff>
--- a/inst/ph_integrated_tables/resources/ph_integrated_template.xlsx
+++ b/inst/ph_integrated_tables/resources/ph_integrated_template.xlsx
@@ -1,33 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Desktop\git\impactR4PHU\inst\ph_integrated_tables\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028A9A9B-2231-44FC-B8BC-5E776486CF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCC5F03-042C-4AD5-9D5C-6E11785C68EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="3" r:id="rId1"/>
     <sheet name="Data" sheetId="1" r:id="rId2"/>
     <sheet name="Cat" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="66">
   <si>
     <t>Impact on Population (Health Outcomes)</t>
   </si>
@@ -50,18 +61,6 @@
     <t>relevant period AMN Phase if available</t>
   </si>
   <si>
-    <t>HH food consumption phase (P3+)</t>
-  </si>
-  <si>
-    <t>% of HHs with poor FCS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of HHs with high rCSI </t>
-  </si>
-  <si>
-    <t>% of HHs with HHS score moderate and above</t>
-  </si>
-  <si>
     <t>Emergency Coping Strategies</t>
   </si>
   <si>
@@ -71,9 +70,6 @@
     <t>Improved Sanitation</t>
   </si>
   <si>
-    <t>Handwashing facilities</t>
-  </si>
-  <si>
     <t>Time to health facilities as per usual mode of transportation (more than 60 min)</t>
   </si>
   <si>
@@ -92,21 +88,12 @@
     <t>Extremely high</t>
   </si>
   <si>
-    <t>&gt;1.4</t>
-  </si>
-  <si>
     <t>&gt; 40%</t>
   </si>
   <si>
     <t>&lt;20%</t>
   </si>
   <si>
-    <t>&gt;80%</t>
-  </si>
-  <si>
-    <t>&gt;40%</t>
-  </si>
-  <si>
     <t>Very high</t>
   </si>
   <si>
@@ -116,15 +103,9 @@
     <t>&gt;30%</t>
   </si>
   <si>
-    <t>P4 IPC AMN</t>
-  </si>
-  <si>
     <t>&lt;40%</t>
   </si>
   <si>
-    <t>&gt;60%</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
@@ -134,9 +115,6 @@
     <t>&gt;20%</t>
   </si>
   <si>
-    <t>P3 IPC AMN</t>
-  </si>
-  <si>
     <t>&lt;60%</t>
   </si>
   <si>
@@ -170,10 +148,94 @@
     <t>&gt;=80%</t>
   </si>
   <si>
-    <t>&lt;=20%</t>
-  </si>
-  <si>
     <t>Improved Water Source</t>
+  </si>
+  <si>
+    <t>&gt;=2</t>
+  </si>
+  <si>
+    <t>&gt; 25%</t>
+  </si>
+  <si>
+    <t>&gt;15%</t>
+  </si>
+  <si>
+    <t>% non-trauma deaths</t>
+  </si>
+  <si>
+    <t>relevant period AFI Phase if available</t>
+  </si>
+  <si>
+    <t>IPC AMN P5</t>
+  </si>
+  <si>
+    <t>IPC AFI 5</t>
+  </si>
+  <si>
+    <t>IPC AMN P4</t>
+  </si>
+  <si>
+    <t>IPC AFI 4</t>
+  </si>
+  <si>
+    <t>IPC AMN P3</t>
+  </si>
+  <si>
+    <t>IPC AFI 3</t>
+  </si>
+  <si>
+    <t>IPC AFI 2</t>
+  </si>
+  <si>
+    <t>IPC AFI 1</t>
+  </si>
+  <si>
+    <t>HH food consumption gap (P3+)</t>
+  </si>
+  <si>
+    <t>Poor FCS</t>
+  </si>
+  <si>
+    <t>High rCSI</t>
+  </si>
+  <si>
+    <t>HHS score severe and very severe</t>
+  </si>
+  <si>
+    <t>&gt; 20%</t>
+  </si>
+  <si>
+    <t>&gt;5%</t>
+  </si>
+  <si>
+    <t>&lt;=5%</t>
+  </si>
+  <si>
+    <t>&gt;8%</t>
+  </si>
+  <si>
+    <t>&gt;6%</t>
+  </si>
+  <si>
+    <t>&gt;4%</t>
+  </si>
+  <si>
+    <t>&lt;=4%</t>
+  </si>
+  <si>
+    <t>Access to handwashing facilities</t>
+  </si>
+  <si>
+    <t>&lt;5%</t>
+  </si>
+  <si>
+    <t>&lt;15%</t>
+  </si>
+  <si>
+    <t>&lt;10%</t>
+  </si>
+  <si>
+    <t>&gt;=20%</t>
   </si>
 </sst>
 </file>
@@ -262,7 +324,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -298,21 +360,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -371,13 +418,130 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -390,19 +554,101 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -411,31 +657,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -444,66 +673,93 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -511,7 +767,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -856,321 +1115,351 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94DF9366-7747-453F-9674-901A9D58CFDA}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="9"/>
-      <c r="B1" s="22" t="s">
+    <row r="1" spans="1:17" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2"/>
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="22" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="1" t="s">
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="34" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="223.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:17" ht="223.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" s="33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="4" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>15</v>
+      <c r="H6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" s="12" t="s">
+    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="B7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="C7" s="12"/>
+      <c r="D7" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="E7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="16" t="s">
+      <c r="G7" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="O5" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="O6" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="K7" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="L7" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="M7" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="N7" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="O7" s="18" t="s">
-        <v>44</v>
+      <c r="N7" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:N1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1178,95 +1467,103 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="22" t="s">
+    <row r="1" spans="1:18" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="22" t="s">
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="1" t="s">
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="34" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="223.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="2" spans="1:18" ht="223.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="N2" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="P2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="Q2" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="R2" s="33" t="s">
         <v>10</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:O1"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="H1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:P2">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
@@ -1291,95 +1588,103 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88864FF9-E532-4B33-9CCF-3B9FDE69E91E}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3:T3"/>
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="22" t="s">
+    <row r="1" spans="1:18" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="22" t="s">
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="1" t="s">
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="34" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="223.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="2" spans="1:18" ht="223.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="N2" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="P2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="Q2" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="R2" s="33" t="s">
         <v>10</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:O1"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="H1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add national level and update individual calculation for unmet healthcare needs (ph_integrated_tables)
</commit_message>
<xml_diff>
--- a/inst/ph_integrated_tables/resources/ph_integrated_template.xlsx
+++ b/inst/ph_integrated_tables/resources/ph_integrated_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Desktop\git\impactR4PHU\inst\ph_integrated_tables\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC11A15F-2E86-4DC6-89CD-57EB3D035F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E861D851-E318-4C3E-8EEA-C8C06BD4AF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1007,37 +1007,37 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1389,7 +1389,7 @@
   <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1479,12 +1479,12 @@
       <c r="B3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="50"/>
+      <c r="C3" s="42"/>
       <c r="D3" s="5" t="s">
         <v>38</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>42</v>
@@ -1522,10 +1522,10 @@
       <c r="Q3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="T3" s="44" t="s">
+      <c r="T3" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="U3" s="45"/>
+      <c r="U3" s="46"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -1534,12 +1534,12 @@
       <c r="B4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="51"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="5" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>44</v>
@@ -1577,8 +1577,8 @@
       <c r="Q4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="T4" s="46"/>
-      <c r="U4" s="47"/>
+      <c r="T4" s="47"/>
+      <c r="U4" s="48"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -1587,12 +1587,12 @@
       <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="51"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="5" t="s">
         <v>39</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>46</v>
@@ -1630,8 +1630,8 @@
       <c r="Q5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="T5" s="46"/>
-      <c r="U5" s="47"/>
+      <c r="T5" s="47"/>
+      <c r="U5" s="48"/>
     </row>
     <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
@@ -1640,7 +1640,7 @@
       <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="51"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="5" t="s">
         <v>28</v>
       </c>
@@ -1683,8 +1683,8 @@
       <c r="Q6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="T6" s="48"/>
-      <c r="U6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="50"/>
     </row>
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
@@ -1693,7 +1693,7 @@
       <c r="B7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="52"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="9" t="s">
         <v>33</v>
       </c>
@@ -1762,10 +1762,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="52"/>
       <c r="C1" s="39" t="s">
         <v>0</v>
       </c>
@@ -1891,22 +1891,22 @@
     </row>
     <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="U11" s="44" t="s">
+      <c r="U11" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="V11" s="45"/>
+      <c r="V11" s="46"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="U12" s="46"/>
-      <c r="V12" s="47"/>
+      <c r="U12" s="47"/>
+      <c r="V12" s="48"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="U13" s="46"/>
-      <c r="V13" s="47"/>
+      <c r="U13" s="47"/>
+      <c r="V13" s="48"/>
     </row>
     <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U14" s="48"/>
-      <c r="V14" s="49"/>
+      <c r="U14" s="49"/>
+      <c r="V14" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1950,10 +1950,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="52"/>
       <c r="C1" s="39" t="s">
         <v>0</v>
       </c>
@@ -2035,22 +2035,22 @@
     </row>
     <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="U4" s="44" t="s">
+      <c r="U4" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="V4" s="45"/>
+      <c r="V4" s="46"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="U5" s="46"/>
-      <c r="V5" s="47"/>
+      <c r="U5" s="47"/>
+      <c r="V5" s="48"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="U6" s="46"/>
-      <c r="V6" s="47"/>
+      <c r="U6" s="47"/>
+      <c r="V6" s="48"/>
     </row>
     <row r="7" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U7" s="48"/>
-      <c r="V7" s="49"/>
+      <c r="U7" s="49"/>
+      <c r="V7" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
add some files images for documentation, fix iycf across library, add ph integrated tables to the documentation
</commit_message>
<xml_diff>
--- a/inst/ph_integrated_tables/resources/ph_integrated_template.xlsx
+++ b/inst/ph_integrated_tables/resources/ph_integrated_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Desktop\git\impactR4PHU\inst\ph_integrated_tables\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E861D851-E318-4C3E-8EEA-C8C06BD4AF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B93F35-B634-40A8-979E-CB9F0049A7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="63">
   <si>
     <t>Impact on Population (Health Outcomes)</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Admin 1</t>
   </si>
   <si>
-    <t>Number of Observation</t>
-  </si>
-  <si>
     <t>Severity level</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
     <t>&gt; 40%</t>
   </si>
   <si>
-    <t>&lt;20%</t>
-  </si>
-  <si>
     <t>Very high</t>
   </si>
   <si>
@@ -103,9 +97,6 @@
     <t>&gt;30%</t>
   </si>
   <si>
-    <t>&lt;40%</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
@@ -115,9 +106,6 @@
     <t>&gt;20%</t>
   </si>
   <si>
-    <t>&lt;60%</t>
-  </si>
-  <si>
     <t>Moderate</t>
   </si>
   <si>
@@ -130,9 +118,6 @@
     <t>IPC AMN P2</t>
   </si>
   <si>
-    <t>&lt;80%</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -145,9 +130,6 @@
     <t>IPC AMN P1</t>
   </si>
   <si>
-    <t>&gt;=80%</t>
-  </si>
-  <si>
     <t>Improved Water Source</t>
   </si>
   <si>
@@ -160,9 +142,6 @@
     <t>&gt;15%</t>
   </si>
   <si>
-    <t>% non-trauma deaths</t>
-  </si>
-  <si>
     <t>relevant period AFI Phase if available</t>
   </si>
   <si>
@@ -223,18 +202,6 @@
     <t>Access to handwashing facilities</t>
   </si>
   <si>
-    <t>&lt;5%</t>
-  </si>
-  <si>
-    <t>&lt;15%</t>
-  </si>
-  <si>
-    <t>&lt;10%</t>
-  </si>
-  <si>
-    <t>&gt;=20%</t>
-  </si>
-  <si>
     <t>HH food consumption gap</t>
   </si>
   <si>
@@ -257,6 +224,9 @@
   </si>
   <si>
     <t>* %s represents non-trauma deaths per admin1 for HH only reporting death</t>
+  </si>
+  <si>
+    <t>Number of Observations</t>
   </si>
 </sst>
 </file>
@@ -1389,7 +1359,7 @@
   <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1421,13 +1391,13 @@
     </row>
     <row r="2" spans="1:21" ht="224.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>4</v>
@@ -1439,25 +1409,25 @@
         <v>6</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="L2" s="21" t="s">
         <v>7</v>
       </c>
       <c r="M2" s="21" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="N2" s="21" t="s">
         <v>8</v>
@@ -1466,275 +1436,245 @@
         <v>9</v>
       </c>
       <c r="P2" s="22" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="Q2" s="26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C3" s="42"/>
       <c r="D3" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="M3" s="5"/>
       <c r="N3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="P3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="5"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="T3" s="45" t="s">
         <v>61</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="T3" s="45" t="s">
-        <v>72</v>
       </c>
       <c r="U3" s="46"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" s="43"/>
       <c r="D4" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="M4" s="5"/>
       <c r="N4" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>63</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="O4" s="5"/>
+      <c r="P4" s="6"/>
       <c r="Q4" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="T4" s="47"/>
       <c r="U4" s="48"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C5" s="43"/>
       <c r="D5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>46</v>
-      </c>
       <c r="G5" s="11" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="H5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="L5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="M5" s="5"/>
       <c r="N5" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>62</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="O5" s="5"/>
+      <c r="P5" s="6"/>
       <c r="Q5" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="T5" s="47"/>
       <c r="U5" s="48"/>
     </row>
     <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C6" s="43"/>
       <c r="D6" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="M6" s="5"/>
       <c r="N6" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>17</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="O6" s="5"/>
+      <c r="P6" s="6"/>
       <c r="Q6" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="T6" s="49"/>
       <c r="U6" s="50"/>
     </row>
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C7" s="44"/>
       <c r="D7" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="M7" s="9"/>
       <c r="N7" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="P7" s="10" t="s">
-        <v>64</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="O7" s="9"/>
+      <c r="P7" s="10"/>
       <c r="Q7" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1753,7 +1693,7 @@
   <dimension ref="A1:V14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U11" sqref="U11:V14"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,13 +1734,13 @@
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>4</v>
@@ -1812,25 +1752,25 @@
         <v>6</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="M2" s="21" t="s">
         <v>7</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="O2" s="21" t="s">
         <v>8</v>
@@ -1839,7 +1779,7 @@
         <v>9</v>
       </c>
       <c r="Q2" s="22" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="R2" s="26" t="s">
         <v>10</v>
@@ -1847,52 +1787,52 @@
     </row>
     <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="U3" s="37" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="V3" s="38" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U4" s="33"/>
       <c r="V4" s="34" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U5" s="28"/>
       <c r="V5" s="35" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U6" s="29"/>
       <c r="V6" s="35" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U7" s="30"/>
       <c r="V7" s="35" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U8" s="31"/>
       <c r="V8" s="35" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="U9" s="32"/>
       <c r="V9" s="36" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U11" s="45" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="V11" s="46"/>
     </row>
@@ -1941,7 +1881,7 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U3" sqref="U3:V6"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1982,13 +1922,13 @@
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>4</v>
@@ -2000,25 +1940,25 @@
         <v>6</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="M2" s="21" t="s">
         <v>7</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="O2" s="21" t="s">
         <v>8</v>
@@ -2027,7 +1967,7 @@
         <v>9</v>
       </c>
       <c r="Q2" s="22" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="R2" s="26" t="s">
         <v>10</v>
@@ -2036,7 +1976,7 @@
     <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U4" s="45" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="V4" s="46"/>
     </row>

</xml_diff>

<commit_message>
small change in title
</commit_message>
<xml_diff>
--- a/inst/ph_integrated_tables/resources/ph_integrated_template.xlsx
+++ b/inst/ph_integrated_tables/resources/ph_integrated_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Desktop\git\impactR4PHU\inst\ph_integrated_tables\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B93F35-B634-40A8-979E-CB9F0049A7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A128763-8087-4853-ABD2-408CF17CE88B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30360" yWindow="1560" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="3" r:id="rId1"/>
@@ -223,10 +223,10 @@
     <t>% non-trauma deaths*</t>
   </si>
   <si>
-    <t>* %s represents non-trauma deaths per admin1 for HH only reporting death</t>
-  </si>
-  <si>
     <t>Number of Observations</t>
+  </si>
+  <si>
+    <t>*non-trauma deaths as percentage of total number of deaths</t>
   </si>
 </sst>
 </file>
@@ -1358,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94DF9366-7747-453F-9674-901A9D58CFDA}">
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,7 +1487,7 @@
         <v>15</v>
       </c>
       <c r="T3" s="45" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U3" s="46"/>
     </row>
@@ -1692,8 +1692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,7 +1734,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>3</v>
@@ -1832,7 +1832,7 @@
     <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U11" s="45" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V11" s="46"/>
     </row>
@@ -1880,8 +1880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88864FF9-E532-4B33-9CCF-3B9FDE69E91E}">
   <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1922,7 +1922,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>3</v>
@@ -1976,7 +1976,7 @@
     <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U4" s="45" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V4" s="46"/>
     </row>

</xml_diff>